<commit_message>
improved admin-orders design and removed all unneсessary promises
</commit_message>
<xml_diff>
--- a/server/files/menu.xlsx
+++ b/server/files/menu.xlsx
@@ -80,7 +80,7 @@
     <t>Дата</t>
   </si>
   <si>
-    <t>23.04.2018-30.04.2018</t>
+    <t>15.07.2018-30.07.2018</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
work in progress, try to limit menu db by 3 elements
</commit_message>
<xml_diff>
--- a/server/files/menu.xlsx
+++ b/server/files/menu.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
   <si>
     <t>пн</t>
   </si>
@@ -80,7 +80,10 @@
     <t>Дата</t>
   </si>
   <si>
-    <t>23.04.2018-30.07.2018</t>
+    <t>супец пупец</t>
+  </si>
+  <si>
+    <t>30.04.2018-30.07.2018</t>
   </si>
 </sst>
 </file>
@@ -409,7 +412,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -423,7 +426,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -437,7 +440,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>350</v>

</xml_diff>

<commit_message>
finally fineshed work with moment.js. thank u a lot my Sanes
</commit_message>
<xml_diff>
--- a/server/files/menu.xlsx
+++ b/server/files/menu.xlsx
@@ -83,7 +83,7 @@
     <t>супец пупец</t>
   </si>
   <si>
-    <t>14.05.2018-30.07.2018</t>
+    <t>30.04.2018-30.07.2018</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
templates statistics 755 otherstuff
</commit_message>
<xml_diff>
--- a/server/files/menu.xlsx
+++ b/server/files/menu.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pavel Ramasheuski\Desktop\EXADEl\Blue\server\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kastu\exadel_repos_blue\mong\server\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3E0893B0-C6AC-410B-8C9B-4F7DBEADCBAD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9380"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -83,13 +84,13 @@
     <t>супец пупец</t>
   </si>
   <si>
-    <t>30.04.2018-30.07.2018</t>
+    <t>21.05.2018-27.05.2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -408,20 +409,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="44.1796875" customWidth="1"/>
-    <col min="3" max="3" width="6.1796875" customWidth="1"/>
+    <col min="2" max="2" width="44.21875" customWidth="1"/>
+    <col min="3" max="3" width="6.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -435,7 +436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -449,7 +450,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -460,7 +461,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -471,7 +472,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -482,7 +483,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -493,7 +494,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -507,7 +508,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -518,7 +519,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -529,7 +530,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -540,7 +541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>5</v>
       </c>
@@ -551,7 +552,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -565,7 +566,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>2</v>
       </c>
@@ -576,7 +577,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>6</v>
       </c>
@@ -587,7 +588,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -598,7 +599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>5</v>
       </c>
@@ -609,7 +610,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -623,7 +624,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>2</v>
       </c>
@@ -634,7 +635,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>6</v>
       </c>
@@ -645,7 +646,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>7</v>
       </c>
@@ -656,7 +657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>5</v>
       </c>
@@ -667,7 +668,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -681,7 +682,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>2</v>
       </c>
@@ -692,7 +693,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>6</v>
       </c>
@@ -703,7 +704,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>7</v>
       </c>
@@ -714,7 +715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>5</v>
       </c>
@@ -725,7 +726,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -739,7 +740,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>2</v>
       </c>
@@ -750,7 +751,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>6</v>
       </c>
@@ -761,7 +762,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>7</v>
       </c>
@@ -772,7 +773,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>5</v>
       </c>
@@ -783,7 +784,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -794,7 +795,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>15</v>
       </c>
@@ -802,7 +803,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>16</v>
       </c>

</xml_diff>